<commit_message>
stupid excel forgot to save the casting the first time!
</commit_message>
<xml_diff>
--- a/20141123_Casting.xlsx
+++ b/20141123_Casting.xlsx
@@ -87,41 +87,41 @@
     <t>Gladius</t>
   </si>
   <si>
-    <t>Morvyn</t>
-  </si>
-  <si>
-    <t>Hermes</t>
-  </si>
-  <si>
-    <t>Caspian</t>
-  </si>
-  <si>
     <t>Jared</t>
   </si>
   <si>
-    <t>Desara</t>
-  </si>
-  <si>
     <t>NPC</t>
   </si>
   <si>
     <t>Waitlist</t>
   </si>
   <si>
-    <t>Valerie</t>
-  </si>
-  <si>
     <t>Pearl</t>
   </si>
   <si>
     <t>Beatrice</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>Mirage</t>
+  </si>
+  <si>
+    <t>Valerian</t>
+  </si>
+  <si>
+    <t>Damien</t>
+  </si>
+  <si>
+    <t>Morgana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,8 +135,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,13 +176,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,13 +504,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -528,7 +530,7 @@
       <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G1" t="s">
@@ -537,102 +539,243 @@
       <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
       <c r="K3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
       <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
       <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="N8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="4"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="4"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -659,34 +802,106 @@
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="6"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
       <c r="O14" s="4"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>